<commit_message>
xls based pricer now passess basic tests and works ass scratching around the plain text parser. this grammar will always be ambiguos even with context sensitivity print formatter fixendorf and co btw office space is a good movie
</commit_message>
<xml_diff>
--- a/test/stock.xlsx
+++ b/test/stock.xlsx
@@ -4,22 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="16020" windowHeight="3060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Romberg es klarika</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>qty</t>
   </si>
@@ -27,9 +24,6 @@
     <t>set</t>
   </si>
   <si>
-    <t>card</t>
-  </si>
-  <si>
     <t>condition</t>
   </si>
   <si>
@@ -54,28 +48,37 @@
     <t>rav</t>
   </si>
   <si>
-    <t>gm</t>
-  </si>
-  <si>
-    <t>Uborka; a tengereszgyalogos</t>
-  </si>
-  <si>
-    <t>Szaponin tabornok</t>
-  </si>
-  <si>
-    <t>Orjongo csigafarm</t>
-  </si>
-  <si>
-    <t>Abbitacel tutajkormany</t>
-  </si>
-  <si>
-    <t>Sargabogre alaku urhajo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alakvalto kocsonya </t>
-  </si>
-  <si>
-    <t>Ex; zsirsertes kiralyfi</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Badlands</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>barrin, master wizard</t>
+  </si>
+  <si>
+    <t>mox jet</t>
+  </si>
+  <si>
+    <t>volcanic island</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>watery grave</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>Power artifact</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,21 +432,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -451,13 +457,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,18 +479,18 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -503,13 +509,13 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,7 +523,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>